<commit_message>
TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_BuyerIsAPotentialRoundTrip - Initial - 9th July 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046981_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheSellsideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367C53EF-6FDA-4727-B86E-218456097CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E9EB0C-3222-4DC2-859C-79F194AFB48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="568" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -378,7 +378,7 @@
     <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
   <si>
-    <t>Requesting to change Company Type to Operating Company with Ownership: Private Equity Group because it is being considered to be a potential round trip.</t>
+    <t>Requesting to change Company Type to Operating Company with Ownership: Private Equity Group because it is being considered to be a potential round trip</t>
   </si>
 </sst>
 </file>
@@ -772,7 +772,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>